<commit_message>
added fixSreadsheet in case any IPUs need to be fixed
</commit_message>
<xml_diff>
--- a/spreadsheets/IPU.xlsx
+++ b/spreadsheets/IPU.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="35" documentId="8_{DD25038B-4C97-4B5C-98E3-067EB3FCA4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA6AB870-AD75-4366-9377-AEABABC3AF21}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="372" windowWidth="20460" windowHeight="11988" xr2:uid="{C38B610A-5224-49A7-99E6-4D31E486AFC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C38B610A-5224-49A7-99E6-4D31E486AFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Clariti 2.0" sheetId="1" r:id="rId1"/>
@@ -1457,8 +1457,8 @@
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
@@ -2408,8 +2408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{415BADD1-1E53-481E-AD09-E640F13A9C7B}">
   <dimension ref="C2:Q9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2489,6 +2489,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006234A633F2607B4AB2F0DD47C854A1A6" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b7f44df6be39d6dfec52f4eeba7d842">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="921a143b-05bd-400c-9eab-f5af2e827b73" xmlns:ns3="82d7a0e6-50aa-4cdc-b5cc-cb9041e495b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d0e2639ea1f75547cde33c72b8f66fac" ns2:_="" ns3:_="">
     <xsd:import namespace="921a143b-05bd-400c-9eab-f5af2e827b73"/>
@@ -2721,15 +2730,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2740,6 +2740,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{245A2814-FEC3-4A50-84E5-3315C1BE1A1E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCC59809-4A3E-4561-B333-E4217FABB892}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2758,14 +2766,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{245A2814-FEC3-4A50-84E5-3315C1BE1A1E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D56CE6C-619A-41F0-899F-103823242E30}">
   <ds:schemaRefs>

</xml_diff>